<commit_message>
Added Configuration (config.properties) file.. Code Updated
</commit_message>
<xml_diff>
--- a/NativeCubeDBMS/sales_datawarehouse.xlsx
+++ b/NativeCubeDBMS/sales_datawarehouse.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="FactTable" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,7 +13,6 @@
     <sheet name="ReportingDate" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Customer" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="SalesPerson" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Sheet6" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="Excel_BuiltIn__FilterDatabase" vbProcedure="false">FactTable!$A$1:$P$50</definedName>
@@ -494,6 +493,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -593,7 +593,7 @@
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -603,7 +603,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="8" style="0" width="11.04"/>
@@ -1908,22 +1908,22 @@
       </c>
       <c r="B2" s="3" t="n">
         <f aca="false">DATE(E2,D2,C2)</f>
-        <v>42011</v>
+        <v>42041</v>
       </c>
       <c r="C2" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F2" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1932,22 +1932,22 @@
       </c>
       <c r="B3" s="3" t="n">
         <f aca="false">DATE(E3,D3,C3)</f>
-        <v>42040</v>
+        <v>42024</v>
       </c>
       <c r="C3" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F3" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1956,22 +1956,22 @@
       </c>
       <c r="B4" s="3" t="n">
         <f aca="false">DATE(E4,D4,C4)</f>
-        <v>42039</v>
+        <v>42079</v>
       </c>
       <c r="C4" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
+        <v>16</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1,3)</f>
+        <v>3</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>2015</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1,7)</f>
         <v>4</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>2015</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1980,22 +1980,22 @@
       </c>
       <c r="B5" s="3" t="n">
         <f aca="false">DATE(E5,D5,C5)</f>
-        <v>42042</v>
+        <v>42015</v>
       </c>
       <c r="C5" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
+        <v>11</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1,3)</f>
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>2015</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1,7)</f>
         <v>7</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>2015</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2004,22 +2004,22 @@
       </c>
       <c r="B6" s="3" t="n">
         <f aca="false">DATE(E6,D6,C6)</f>
-        <v>42007</v>
+        <v>42075</v>
       </c>
       <c r="C6" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F6" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2028,22 +2028,22 @@
       </c>
       <c r="B7" s="3" t="n">
         <f aca="false">DATE(E7,D7,C7)</f>
-        <v>42021</v>
+        <v>42059</v>
       </c>
       <c r="C7" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F7" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2052,22 +2052,22 @@
       </c>
       <c r="B8" s="3" t="n">
         <f aca="false">DATE(E8,D8,C8)</f>
-        <v>42068</v>
+        <v>42019</v>
       </c>
       <c r="C8" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D8" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F8" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2091,7 +2091,7 @@
       </c>
       <c r="F9" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2100,11 +2100,11 @@
       </c>
       <c r="B10" s="3" t="n">
         <f aca="false">DATE(E10,D10,C10)</f>
-        <v>42040</v>
+        <v>42049</v>
       </c>
       <c r="C10" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D10" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="F10" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2124,22 +2124,22 @@
       </c>
       <c r="B11" s="3" t="n">
         <f aca="false">DATE(E11,D11,C11)</f>
-        <v>42073</v>
+        <v>42036</v>
       </c>
       <c r="C11" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F11" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2148,22 +2148,22 @@
       </c>
       <c r="B12" s="3" t="n">
         <f aca="false">DATE(E12,D12,C12)</f>
-        <v>42010</v>
+        <v>42060</v>
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F12" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2172,22 +2172,22 @@
       </c>
       <c r="B13" s="3" t="n">
         <f aca="false">DATE(E13,D13,C13)</f>
-        <v>42047</v>
+        <v>42092</v>
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="D13" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F13" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2196,11 +2196,11 @@
       </c>
       <c r="B14" s="3" t="n">
         <f aca="false">DATE(E14,D14,C14)</f>
-        <v>42088</v>
+        <v>42084</v>
       </c>
       <c r="C14" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="F14" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2220,15 +2220,15 @@
       </c>
       <c r="B15" s="3" t="n">
         <f aca="false">DATE(E15,D15,C15)</f>
-        <v>42060</v>
+        <v>42069</v>
       </c>
       <c r="C15" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D15" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>2015</v>
@@ -2244,11 +2244,11 @@
       </c>
       <c r="B16" s="3" t="n">
         <f aca="false">DATE(E16,D16,C16)</f>
-        <v>42077</v>
+        <v>42086</v>
       </c>
       <c r="C16" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D16" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -2259,7 +2259,7 @@
       </c>
       <c r="F16" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2268,22 +2268,22 @@
       </c>
       <c r="B17" s="3" t="n">
         <f aca="false">DATE(E17,D17,C17)</f>
-        <v>42048</v>
+        <v>42016</v>
       </c>
       <c r="C17" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F17" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2292,22 +2292,22 @@
       </c>
       <c r="B18" s="3" t="n">
         <f aca="false">DATE(E18,D18,C18)</f>
-        <v>42023</v>
+        <v>42053</v>
       </c>
       <c r="C18" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F18" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2316,11 +2316,11 @@
       </c>
       <c r="B19" s="3" t="n">
         <f aca="false">DATE(E19,D19,C19)</f>
-        <v>42055</v>
+        <v>42047</v>
       </c>
       <c r="C19" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D19" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -2331,7 +2331,7 @@
       </c>
       <c r="F19" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2340,11 +2340,11 @@
       </c>
       <c r="B20" s="3" t="n">
         <f aca="false">DATE(E20,D20,C20)</f>
-        <v>42021</v>
+        <v>42006</v>
       </c>
       <c r="C20" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D20" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -2355,7 +2355,7 @@
       </c>
       <c r="F20" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2364,15 +2364,15 @@
       </c>
       <c r="B21" s="3" t="n">
         <f aca="false">DATE(E21,D21,C21)</f>
-        <v>42046</v>
+        <v>42089</v>
       </c>
       <c r="C21" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D21" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>2015</v>
@@ -2388,22 +2388,22 @@
       </c>
       <c r="B22" s="3" t="n">
         <f aca="false">DATE(E22,D22,C22)</f>
-        <v>42093</v>
+        <v>42057</v>
       </c>
       <c r="C22" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D22" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F22" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2412,11 +2412,11 @@
       </c>
       <c r="B23" s="3" t="n">
         <f aca="false">DATE(E23,D23,C23)</f>
-        <v>42072</v>
+        <v>42090</v>
       </c>
       <c r="C23" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="D23" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -2427,7 +2427,7 @@
       </c>
       <c r="F23" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2436,15 +2436,15 @@
       </c>
       <c r="B24" s="3" t="n">
         <f aca="false">DATE(E24,D24,C24)</f>
-        <v>42092</v>
+        <v>42040</v>
       </c>
       <c r="C24" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="D24" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>2015</v>
@@ -2460,11 +2460,11 @@
       </c>
       <c r="B25" s="3" t="n">
         <f aca="false">DATE(E25,D25,C25)</f>
-        <v>42034</v>
+        <v>42017</v>
       </c>
       <c r="C25" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D25" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -2475,7 +2475,7 @@
       </c>
       <c r="F25" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2484,15 +2484,15 @@
       </c>
       <c r="B26" s="3" t="n">
         <f aca="false">DATE(E26,D26,C26)</f>
-        <v>42070</v>
+        <v>42024</v>
       </c>
       <c r="C26" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D26" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>2015</v>
@@ -2508,15 +2508,15 @@
       </c>
       <c r="B27" s="3" t="n">
         <f aca="false">DATE(E27,D27,C27)</f>
-        <v>42070</v>
+        <v>42058</v>
       </c>
       <c r="C27" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D27" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>2015</v>
@@ -2532,22 +2532,22 @@
       </c>
       <c r="B28" s="3" t="n">
         <f aca="false">DATE(E28,D28,C28)</f>
-        <v>42028</v>
+        <v>42060</v>
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D28" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F28" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2556,22 +2556,22 @@
       </c>
       <c r="B29" s="3" t="n">
         <f aca="false">DATE(E29,D29,C29)</f>
-        <v>42074</v>
+        <v>42053</v>
       </c>
       <c r="C29" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D29" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F29" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2580,22 +2580,22 @@
       </c>
       <c r="B30" s="3" t="n">
         <f aca="false">DATE(E30,D30,C30)</f>
-        <v>42024</v>
+        <v>42089</v>
       </c>
       <c r="C30" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D30" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F30" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2604,7 +2604,7 @@
       </c>
       <c r="B31" s="3" t="n">
         <f aca="false">DATE(E31,D31,C31)</f>
-        <v>42047</v>
+        <v>42075</v>
       </c>
       <c r="C31" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
@@ -2612,14 +2612,14 @@
       </c>
       <c r="D31" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F31" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2628,22 +2628,22 @@
       </c>
       <c r="B32" s="3" t="n">
         <f aca="false">DATE(E32,D32,C32)</f>
-        <v>42023</v>
+        <v>42075</v>
       </c>
       <c r="C32" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D32" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F32" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2652,22 +2652,22 @@
       </c>
       <c r="B33" s="3" t="n">
         <f aca="false">DATE(E33,D33,C33)</f>
-        <v>42065</v>
+        <v>42025</v>
       </c>
       <c r="C33" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D33" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F33" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2676,11 +2676,11 @@
       </c>
       <c r="B34" s="3" t="n">
         <f aca="false">DATE(E34,D34,C34)</f>
-        <v>42073</v>
+        <v>42069</v>
       </c>
       <c r="C34" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D34" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -2691,7 +2691,7 @@
       </c>
       <c r="F34" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2700,11 +2700,11 @@
       </c>
       <c r="B35" s="3" t="n">
         <f aca="false">DATE(E35,D35,C35)</f>
-        <v>42044</v>
+        <v>42053</v>
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D35" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -2715,7 +2715,7 @@
       </c>
       <c r="F35" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2724,22 +2724,22 @@
       </c>
       <c r="B36" s="3" t="n">
         <f aca="false">DATE(E36,D36,C36)</f>
-        <v>42054</v>
+        <v>42025</v>
       </c>
       <c r="C36" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D36" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F36" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2763,7 +2763,7 @@
       </c>
       <c r="F37" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2772,22 +2772,22 @@
       </c>
       <c r="B38" s="3" t="n">
         <f aca="false">DATE(E38,D38,C38)</f>
-        <v>42006</v>
+        <v>42039</v>
       </c>
       <c r="C38" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D38" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F38" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2796,22 +2796,22 @@
       </c>
       <c r="B39" s="3" t="n">
         <f aca="false">DATE(E39,D39,C39)</f>
-        <v>42056</v>
+        <v>42013</v>
       </c>
       <c r="C39" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D39" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F39" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2820,7 +2820,7 @@
       </c>
       <c r="B40" s="3" t="n">
         <f aca="false">DATE(E40,D40,C40)</f>
-        <v>42020</v>
+        <v>42079</v>
       </c>
       <c r="C40" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
@@ -2828,14 +2828,14 @@
       </c>
       <c r="D40" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E40" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F40" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2844,22 +2844,22 @@
       </c>
       <c r="B41" s="3" t="n">
         <f aca="false">DATE(E41,D41,C41)</f>
-        <v>42034</v>
+        <v>42089</v>
       </c>
       <c r="C41" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D41" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E41" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F41" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2868,22 +2868,22 @@
       </c>
       <c r="B42" s="3" t="n">
         <f aca="false">DATE(E42,D42,C42)</f>
-        <v>42023</v>
+        <v>42079</v>
       </c>
       <c r="C42" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D42" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E42" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F42" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2892,22 +2892,22 @@
       </c>
       <c r="B43" s="3" t="n">
         <f aca="false">DATE(E43,D43,C43)</f>
-        <v>42036</v>
+        <v>42066</v>
       </c>
       <c r="C43" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D43" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E43" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F43" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2916,22 +2916,22 @@
       </c>
       <c r="B44" s="3" t="n">
         <f aca="false">DATE(E44,D44,C44)</f>
-        <v>42009</v>
+        <v>42056</v>
       </c>
       <c r="C44" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D44" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F44" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2940,11 +2940,11 @@
       </c>
       <c r="B45" s="3" t="n">
         <f aca="false">DATE(E45,D45,C45)</f>
-        <v>42075</v>
+        <v>42064</v>
       </c>
       <c r="C45" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D45" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -2955,7 +2955,7 @@
       </c>
       <c r="F45" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2964,11 +2964,11 @@
       </c>
       <c r="B46" s="3" t="n">
         <f aca="false">DATE(E46,D46,C46)</f>
-        <v>42015</v>
+        <v>42009</v>
       </c>
       <c r="C46" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D46" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -2979,7 +2979,7 @@
       </c>
       <c r="F46" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2988,22 +2988,22 @@
       </c>
       <c r="B47" s="3" t="n">
         <f aca="false">DATE(E47,D47,C47)</f>
-        <v>42037</v>
+        <v>42023</v>
       </c>
       <c r="C47" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D47" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E47" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F47" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3012,15 +3012,15 @@
       </c>
       <c r="B48" s="3" t="n">
         <f aca="false">DATE(E48,D48,C48)</f>
-        <v>42025</v>
+        <v>42086</v>
       </c>
       <c r="C48" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D48" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E48" s="0" t="n">
         <v>2015</v>
@@ -3036,22 +3036,22 @@
       </c>
       <c r="B49" s="3" t="n">
         <f aca="false">DATE(E49,D49,C49)</f>
-        <v>42092</v>
+        <v>42027</v>
       </c>
       <c r="C49" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D49" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E49" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F49" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3060,22 +3060,22 @@
       </c>
       <c r="B50" s="3" t="n">
         <f aca="false">DATE(E50,D50,C50)</f>
-        <v>42006</v>
+        <v>42078</v>
       </c>
       <c r="C50" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D50" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E50" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F50" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3084,22 +3084,22 @@
       </c>
       <c r="B51" s="3" t="n">
         <f aca="false">DATE(E51,D51,C51)</f>
-        <v>42051</v>
+        <v>42023</v>
       </c>
       <c r="C51" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D51" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E51" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F51" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3108,22 +3108,22 @@
       </c>
       <c r="B52" s="3" t="n">
         <f aca="false">DATE(E52,D52,C52)</f>
-        <v>42087</v>
+        <v>42058</v>
       </c>
       <c r="C52" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D52" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E52" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F52" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3132,15 +3132,15 @@
       </c>
       <c r="B53" s="3" t="n">
         <f aca="false">DATE(E53,D53,C53)</f>
-        <v>42028</v>
+        <v>42054</v>
       </c>
       <c r="C53" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D53" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E53" s="0" t="n">
         <v>2015</v>
@@ -3156,22 +3156,22 @@
       </c>
       <c r="B54" s="3" t="n">
         <f aca="false">DATE(E54,D54,C54)</f>
-        <v>42039</v>
+        <v>42020</v>
       </c>
       <c r="C54" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D54" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E54" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F54" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3180,22 +3180,22 @@
       </c>
       <c r="B55" s="3" t="n">
         <f aca="false">DATE(E55,D55,C55)</f>
-        <v>42085</v>
+        <v>42037</v>
       </c>
       <c r="C55" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D55" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E55" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F55" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3204,22 +3204,22 @@
       </c>
       <c r="B56" s="3" t="n">
         <f aca="false">DATE(E56,D56,C56)</f>
-        <v>42037</v>
+        <v>42017</v>
       </c>
       <c r="C56" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D56" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E56" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F56" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3228,11 +3228,11 @@
       </c>
       <c r="B57" s="3" t="n">
         <f aca="false">DATE(E57,D57,C57)</f>
-        <v>42083</v>
+        <v>42081</v>
       </c>
       <c r="C57" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D57" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -3243,7 +3243,7 @@
       </c>
       <c r="F57" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3252,11 +3252,11 @@
       </c>
       <c r="B58" s="3" t="n">
         <f aca="false">DATE(E58,D58,C58)</f>
-        <v>42013</v>
+        <v>42029</v>
       </c>
       <c r="C58" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D58" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -3267,7 +3267,7 @@
       </c>
       <c r="F58" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3276,11 +3276,11 @@
       </c>
       <c r="B59" s="3" t="n">
         <f aca="false">DATE(E59,D59,C59)</f>
-        <v>42053</v>
+        <v>42050</v>
       </c>
       <c r="C59" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D59" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -3291,7 +3291,7 @@
       </c>
       <c r="F59" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3300,22 +3300,22 @@
       </c>
       <c r="B60" s="3" t="n">
         <f aca="false">DATE(E60,D60,C60)</f>
-        <v>42071</v>
+        <v>42048</v>
       </c>
       <c r="C60" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D60" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E60" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F60" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3339,7 +3339,7 @@
       </c>
       <c r="F61" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3348,22 +3348,22 @@
       </c>
       <c r="B62" s="3" t="n">
         <f aca="false">DATE(E62,D62,C62)</f>
-        <v>42085</v>
+        <v>42055</v>
       </c>
       <c r="C62" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D62" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E62" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F62" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3372,22 +3372,22 @@
       </c>
       <c r="B63" s="3" t="n">
         <f aca="false">DATE(E63,D63,C63)</f>
-        <v>42080</v>
+        <v>42018</v>
       </c>
       <c r="C63" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D63" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E63" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F63" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3396,11 +3396,11 @@
       </c>
       <c r="B64" s="3" t="n">
         <f aca="false">DATE(E64,D64,C64)</f>
-        <v>42019</v>
+        <v>42006</v>
       </c>
       <c r="C64" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D64" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -3411,7 +3411,7 @@
       </c>
       <c r="F64" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3420,22 +3420,22 @@
       </c>
       <c r="B65" s="3" t="n">
         <f aca="false">DATE(E65,D65,C65)</f>
-        <v>42020</v>
+        <v>42037</v>
       </c>
       <c r="C65" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D65" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E65" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F65" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3444,22 +3444,22 @@
       </c>
       <c r="B66" s="3" t="n">
         <f aca="false">DATE(E66,D66,C66)</f>
-        <v>42008</v>
+        <v>42092</v>
       </c>
       <c r="C66" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="D66" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E66" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F66" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3468,22 +3468,22 @@
       </c>
       <c r="B67" s="3" t="n">
         <f aca="false">DATE(E67,D67,C67)</f>
-        <v>42060</v>
+        <v>42026</v>
       </c>
       <c r="C67" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D67" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E67" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F67" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3492,22 +3492,22 @@
       </c>
       <c r="B68" s="3" t="n">
         <f aca="false">DATE(E68,D68,C68)</f>
-        <v>42009</v>
+        <v>42063</v>
       </c>
       <c r="C68" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D68" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E68" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F68" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3516,11 +3516,11 @@
       </c>
       <c r="B69" s="3" t="n">
         <f aca="false">DATE(E69,D69,C69)</f>
-        <v>42054</v>
+        <v>42041</v>
       </c>
       <c r="C69" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D69" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -3531,7 +3531,7 @@
       </c>
       <c r="F69" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3540,22 +3540,22 @@
       </c>
       <c r="B70" s="3" t="n">
         <f aca="false">DATE(E70,D70,C70)</f>
-        <v>42013</v>
+        <v>42089</v>
       </c>
       <c r="C70" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D70" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E70" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F70" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3564,22 +3564,22 @@
       </c>
       <c r="B71" s="3" t="n">
         <f aca="false">DATE(E71,D71,C71)</f>
-        <v>42066</v>
+        <v>42006</v>
       </c>
       <c r="C71" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D71" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E71" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F71" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3588,11 +3588,11 @@
       </c>
       <c r="B72" s="3" t="n">
         <f aca="false">DATE(E72,D72,C72)</f>
-        <v>42027</v>
+        <v>42015</v>
       </c>
       <c r="C72" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D72" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -3603,7 +3603,7 @@
       </c>
       <c r="F72" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3612,11 +3612,11 @@
       </c>
       <c r="B73" s="3" t="n">
         <f aca="false">DATE(E73,D73,C73)</f>
-        <v>42037</v>
+        <v>42063</v>
       </c>
       <c r="C73" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="D73" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -3627,7 +3627,7 @@
       </c>
       <c r="F73" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3636,11 +3636,11 @@
       </c>
       <c r="B74" s="3" t="n">
         <f aca="false">DATE(E74,D74,C74)</f>
-        <v>42030</v>
+        <v>42008</v>
       </c>
       <c r="C74" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="D74" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -3660,11 +3660,11 @@
       </c>
       <c r="B75" s="3" t="n">
         <f aca="false">DATE(E75,D75,C75)</f>
-        <v>42091</v>
+        <v>42086</v>
       </c>
       <c r="C75" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D75" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="F75" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3684,22 +3684,22 @@
       </c>
       <c r="B76" s="3" t="n">
         <f aca="false">DATE(E76,D76,C76)</f>
-        <v>42022</v>
+        <v>42068</v>
       </c>
       <c r="C76" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D76" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E76" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F76" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3708,11 +3708,11 @@
       </c>
       <c r="B77" s="3" t="n">
         <f aca="false">DATE(E77,D77,C77)</f>
-        <v>42067</v>
+        <v>42085</v>
       </c>
       <c r="C77" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D77" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -3732,7 +3732,7 @@
       </c>
       <c r="B78" s="3" t="n">
         <f aca="false">DATE(E78,D78,C78)</f>
-        <v>42066</v>
+        <v>42038</v>
       </c>
       <c r="C78" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
@@ -3740,14 +3740,14 @@
       </c>
       <c r="D78" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E78" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F78" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3756,22 +3756,22 @@
       </c>
       <c r="B79" s="3" t="n">
         <f aca="false">DATE(E79,D79,C79)</f>
-        <v>42049</v>
+        <v>42034</v>
       </c>
       <c r="C79" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="D79" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E79" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F79" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3780,22 +3780,22 @@
       </c>
       <c r="B80" s="3" t="n">
         <f aca="false">DATE(E80,D80,C80)</f>
-        <v>42020</v>
+        <v>42042</v>
       </c>
       <c r="C80" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D80" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E80" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F80" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3804,11 +3804,11 @@
       </c>
       <c r="B81" s="3" t="n">
         <f aca="false">DATE(E81,D81,C81)</f>
-        <v>42067</v>
+        <v>42077</v>
       </c>
       <c r="C81" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D81" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -3828,22 +3828,22 @@
       </c>
       <c r="B82" s="3" t="n">
         <f aca="false">DATE(E82,D82,C82)</f>
-        <v>42054</v>
+        <v>42086</v>
       </c>
       <c r="C82" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D82" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E82" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F82" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3852,11 +3852,11 @@
       </c>
       <c r="B83" s="3" t="n">
         <f aca="false">DATE(E83,D83,C83)</f>
-        <v>42080</v>
+        <v>42073</v>
       </c>
       <c r="C83" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D83" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -3867,7 +3867,7 @@
       </c>
       <c r="F83" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3876,11 +3876,11 @@
       </c>
       <c r="B84" s="3" t="n">
         <f aca="false">DATE(E84,D84,C84)</f>
-        <v>42082</v>
+        <v>42086</v>
       </c>
       <c r="C84" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D84" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -3891,7 +3891,7 @@
       </c>
       <c r="F84" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3900,15 +3900,15 @@
       </c>
       <c r="B85" s="3" t="n">
         <f aca="false">DATE(E85,D85,C85)</f>
-        <v>42082</v>
+        <v>42055</v>
       </c>
       <c r="C85" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D85" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E85" s="0" t="n">
         <v>2015</v>
@@ -3924,22 +3924,22 @@
       </c>
       <c r="B86" s="3" t="n">
         <f aca="false">DATE(E86,D86,C86)</f>
-        <v>42078</v>
+        <v>42062</v>
       </c>
       <c r="C86" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D86" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E86" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F86" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3948,22 +3948,22 @@
       </c>
       <c r="B87" s="3" t="n">
         <f aca="false">DATE(E87,D87,C87)</f>
-        <v>42022</v>
+        <v>42056</v>
       </c>
       <c r="C87" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D87" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E87" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F87" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3972,11 +3972,11 @@
       </c>
       <c r="B88" s="3" t="n">
         <f aca="false">DATE(E88,D88,C88)</f>
-        <v>42046</v>
+        <v>42044</v>
       </c>
       <c r="C88" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D88" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -3987,7 +3987,7 @@
       </c>
       <c r="F88" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3996,11 +3996,11 @@
       </c>
       <c r="B89" s="3" t="n">
         <f aca="false">DATE(E89,D89,C89)</f>
-        <v>42071</v>
+        <v>42080</v>
       </c>
       <c r="C89" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D89" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -4011,7 +4011,7 @@
       </c>
       <c r="F89" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4020,11 +4020,11 @@
       </c>
       <c r="B90" s="3" t="n">
         <f aca="false">DATE(E90,D90,C90)</f>
-        <v>42016</v>
+        <v>42022</v>
       </c>
       <c r="C90" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D90" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -4044,11 +4044,11 @@
       </c>
       <c r="B91" s="3" t="n">
         <f aca="false">DATE(E91,D91,C91)</f>
-        <v>42083</v>
+        <v>42088</v>
       </c>
       <c r="C91" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D91" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -4059,7 +4059,7 @@
       </c>
       <c r="F91" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4068,22 +4068,22 @@
       </c>
       <c r="B92" s="3" t="n">
         <f aca="false">DATE(E92,D92,C92)</f>
-        <v>42012</v>
+        <v>42040</v>
       </c>
       <c r="C92" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D92" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E92" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F92" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4092,11 +4092,11 @@
       </c>
       <c r="B93" s="3" t="n">
         <f aca="false">DATE(E93,D93,C93)</f>
-        <v>42074</v>
+        <v>42090</v>
       </c>
       <c r="C93" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D93" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -4107,7 +4107,7 @@
       </c>
       <c r="F93" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4116,15 +4116,15 @@
       </c>
       <c r="B94" s="3" t="n">
         <f aca="false">DATE(E94,D94,C94)</f>
-        <v>42082</v>
+        <v>42050</v>
       </c>
       <c r="C94" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D94" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E94" s="0" t="n">
         <v>2015</v>
@@ -4140,22 +4140,22 @@
       </c>
       <c r="B95" s="3" t="n">
         <f aca="false">DATE(E95,D95,C95)</f>
-        <v>42074</v>
+        <v>42041</v>
       </c>
       <c r="C95" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D95" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E95" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F95" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4164,11 +4164,11 @@
       </c>
       <c r="B96" s="3" t="n">
         <f aca="false">DATE(E96,D96,C96)</f>
-        <v>42061</v>
+        <v>42045</v>
       </c>
       <c r="C96" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D96" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -4179,7 +4179,7 @@
       </c>
       <c r="F96" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4188,11 +4188,11 @@
       </c>
       <c r="B97" s="3" t="n">
         <f aca="false">DATE(E97,D97,C97)</f>
-        <v>42072</v>
+        <v>42092</v>
       </c>
       <c r="C97" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="D97" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -4203,7 +4203,7 @@
       </c>
       <c r="F97" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4212,11 +4212,11 @@
       </c>
       <c r="B98" s="3" t="n">
         <f aca="false">DATE(E98,D98,C98)</f>
-        <v>42043</v>
+        <v>42061</v>
       </c>
       <c r="C98" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D98" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -4236,11 +4236,11 @@
       </c>
       <c r="B99" s="3" t="n">
         <f aca="false">DATE(E99,D99,C99)</f>
-        <v>42052</v>
+        <v>42038</v>
       </c>
       <c r="C99" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="D99" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -4251,7 +4251,7 @@
       </c>
       <c r="F99" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4260,22 +4260,22 @@
       </c>
       <c r="B100" s="3" t="n">
         <f aca="false">DATE(E100,D100,C100)</f>
-        <v>42069</v>
+        <v>42053</v>
       </c>
       <c r="C100" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D100" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E100" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="F100" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4284,11 +4284,11 @@
       </c>
       <c r="B101" s="3" t="n">
         <f aca="false">DATE(E101,D101,C101)</f>
-        <v>42089</v>
+        <v>42088</v>
       </c>
       <c r="C101" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,30)</f>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D101" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
@@ -4299,7 +4299,7 @@
       </c>
       <c r="F101" s="0" t="n">
         <f aca="false">RANDBETWEEN(1,7)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -4416,7 +4416,7 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -4503,30 +4503,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.04"/>
-  </cols>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>